<commit_message>
tried and removed wedge case Z, need to run A for ThO2
</commit_message>
<xml_diff>
--- a/Jupyter/Wedge/wedge_data_2025-12-31.xlsx
+++ b/Jupyter/Wedge/wedge_data_2025-12-31.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\Jupyter\Wedge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD651A76-9F79-446A-8364-60A05ED5CF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA05213-BEA7-4978-A3AA-349D2210DDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-36" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fissile production" sheetId="2" r:id="rId1"/>
@@ -184,7 +184,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -334,8 +334,8 @@
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2537,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FC2A7-2007-48F8-8A3D-08B47124466B}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4869,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22416C2-1180-4450-A3B0-0B08DD9AEC85}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5079,30 +5079,26 @@
         <v>29.746282999999998</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="27">
-        <v>3.52725672373683E-5</v>
-      </c>
-      <c r="I10" s="22">
-        <v>3.4271699999999999E-5</v>
-      </c>
-      <c r="J10" s="2">
-        <v>3.4428100000000003E-5</v>
-      </c>
-      <c r="K10" s="2">
-        <f>P10*$T$3*$W$3*1E-24</f>
-        <v>3.4288459937199994E-5</v>
-      </c>
+      <c r="H10">
+        <v>1.40420707746021</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="32">
+        <f>1.35286+0.0130625</f>
+        <v>1.3659224999999999</v>
+      </c>
+      <c r="K10" s="2"/>
       <c r="L10" s="11">
         <f t="shared" ref="L10:L22" si="1">I10/H10</f>
-        <v>0.97162476916882967</v>
+        <v>0</v>
       </c>
       <c r="M10" s="11">
         <f t="shared" ref="M10:M22" si="2">J10/H10</f>
-        <v>0.97605880990500582</v>
+        <v>0.97273580366119827</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" ref="N10:N22" si="3">K10/H10</f>
-        <v>0.97209992418341107</v>
+        <v>0</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="2">
@@ -5130,30 +5126,26 @@
         <v>13.302942</v>
       </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="28">
-        <v>1.76088265923015E-4</v>
-      </c>
-      <c r="I11" s="26">
-        <v>1.7047000000000001E-4</v>
-      </c>
-      <c r="J11" s="5">
-        <v>1.7116899999999999E-4</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" ref="K11:K22" si="4">P11*$T$3*$W$3*1E-24</f>
-        <v>1.7111952961599997E-4</v>
-      </c>
+      <c r="H11" s="4">
+        <v>1.4042408208581401</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="33">
+        <f>1.35209+ 0.0130713</f>
+        <v>1.3651613</v>
+      </c>
+      <c r="K11" s="5"/>
       <c r="L11" s="9">
         <f t="shared" si="1"/>
-        <v>0.96809403571802299</v>
+        <v>0</v>
       </c>
       <c r="M11" s="9">
         <f t="shared" si="2"/>
-        <v>0.97206363582928523</v>
+        <v>0.97217035690911024</v>
       </c>
       <c r="N11" s="9">
         <f t="shared" si="3"/>
-        <v>0.9717826949969095</v>
+        <v>0</v>
       </c>
       <c r="P11" s="5">
         <v>1.36516E-2</v>
@@ -5181,30 +5173,26 @@
         <v>7.6804569999999996</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="27">
-        <v>5.2684723504348998E-4</v>
-      </c>
-      <c r="I12" s="22">
-        <v>5.1337799999999999E-4</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5.1237400000000001E-4</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="4"/>
-        <v>5.1184438984000003E-4</v>
-      </c>
+      <c r="H12">
+        <v>1.4037049162311801</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="32">
+        <f>1.35042+0.0130583</f>
+        <v>1.3634782999999999</v>
+      </c>
+      <c r="K12" s="2"/>
       <c r="L12" s="11">
         <f t="shared" si="1"/>
-        <v>0.97443426832755775</v>
+        <v>0</v>
       </c>
       <c r="M12" s="11">
         <f t="shared" si="2"/>
-        <v>0.97252859257713431</v>
+        <v>0.97134254089585648</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" si="3"/>
-        <v>0.97152334831509268</v>
+        <v>0</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="2">
@@ -5232,30 +5220,26 @@
         <v>2.4287740000000002</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="28">
-        <v>5.02535867346246E-3</v>
-      </c>
-      <c r="I13" s="26">
-        <v>4.8983400000000002E-3</v>
-      </c>
-      <c r="J13" s="5">
-        <v>4.8734900000000003E-3</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="4"/>
-        <v>4.88413162972E-3</v>
-      </c>
+      <c r="H13" s="4">
+        <v>1.3978225806626601</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="33">
+        <f xml:space="preserve"> 1.3458+ 0.0130269</f>
+        <v>1.3588269000000002</v>
+      </c>
+      <c r="K13" s="5"/>
       <c r="L13" s="9">
         <f t="shared" si="1"/>
-        <v>0.97472445616007264</v>
+        <v>0</v>
       </c>
       <c r="M13" s="9">
         <f t="shared" si="2"/>
-        <v>0.96977953548580786</v>
+        <v>0.97210255349847519</v>
       </c>
       <c r="N13" s="9">
         <f t="shared" si="3"/>
-        <v>0.97189712159487418</v>
+        <v>0</v>
       </c>
       <c r="P13" s="5">
         <v>0.38964700000000002</v>
@@ -5283,30 +5267,26 @@
         <v>1.7174020000000001</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="27">
-        <v>9.6096776712520909E-3</v>
-      </c>
-      <c r="I14" s="22">
-        <v>9.3411799999999993E-3</v>
-      </c>
-      <c r="J14" s="2">
-        <v>9.3206399999999998E-3</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="4"/>
-        <v>9.338383665239999E-3</v>
-      </c>
+      <c r="H14">
+        <v>1.3935791421766499</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="32">
+        <f xml:space="preserve"> 1.34161+ 0.0129693</f>
+        <v>1.3545792999999999</v>
+      </c>
+      <c r="K14" s="2"/>
       <c r="L14" s="11">
         <f t="shared" si="1"/>
-        <v>0.97205965897739544</v>
+        <v>0</v>
       </c>
       <c r="M14" s="11">
         <f t="shared" si="2"/>
-        <v>0.9699222303660856</v>
+        <v>0.97201461976839321</v>
       </c>
       <c r="N14" s="11">
         <f t="shared" si="3"/>
-        <v>0.97176866745242829</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="2">
@@ -5334,30 +5314,26 @@
         <v>1.2143870000000001</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="28">
-        <v>1.7956202904139199E-2</v>
-      </c>
-      <c r="I15" s="26">
-        <v>1.7297199999999999E-2</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1.75224E-2</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="4"/>
-        <v>1.7408149340399998E-2</v>
-      </c>
+      <c r="H15" s="4">
+        <v>1.38536063754419</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="33">
+        <f xml:space="preserve"> 1.33559+ 0.012842</f>
+        <v>1.3484320000000001</v>
+      </c>
+      <c r="K15" s="5"/>
       <c r="L15" s="9">
         <f t="shared" si="1"/>
-        <v>0.96329942874574614</v>
+        <v>0</v>
       </c>
       <c r="M15" s="9">
         <f t="shared" si="2"/>
-        <v>0.97584105579252511</v>
+        <v>0.973343664787782</v>
       </c>
       <c r="N15" s="9">
         <f t="shared" si="3"/>
-        <v>0.96947831528385853</v>
+        <v>0</v>
       </c>
       <c r="P15" s="5">
         <v>1.38879</v>
@@ -5385,30 +5361,26 @@
         <v>0.99154299999999995</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="27">
-        <v>2.54716677488637E-2</v>
-      </c>
-      <c r="I16" s="22">
-        <v>2.4680299999999999E-2</v>
-      </c>
-      <c r="J16" s="2">
-        <v>2.4773900000000001E-2</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="4"/>
-        <v>2.4696861585199997E-2</v>
-      </c>
+      <c r="H16">
+        <v>1.37856347972413</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="32">
+        <f xml:space="preserve"> 1.32652+0.0127696</f>
+        <v>1.3392895999999999</v>
+      </c>
+      <c r="K16" s="2"/>
       <c r="L16" s="11">
         <f t="shared" si="1"/>
-        <v>0.96893145134169689</v>
+        <v>0</v>
       </c>
       <c r="M16" s="11">
         <f t="shared" si="2"/>
-        <v>0.97260612238887156</v>
+        <v>0.97151101106204452</v>
       </c>
       <c r="N16" s="11">
         <f t="shared" si="3"/>
-        <v>0.9695816476838951</v>
+        <v>0</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="2">
@@ -5436,30 +5408,26 @@
         <v>0.85870100000000005</v>
       </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="28">
-        <v>3.2417642839879697E-2</v>
-      </c>
-      <c r="I17" s="26">
-        <v>3.15217E-2</v>
-      </c>
-      <c r="J17" s="5">
-        <v>3.1542500000000001E-2</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="4"/>
-        <v>3.1496843537600003E-2</v>
-      </c>
+      <c r="H17" s="4">
+        <v>1.3699400435562701</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="33">
+        <f xml:space="preserve"> 1.31981+0.0126516</f>
+        <v>1.3324616</v>
+      </c>
+      <c r="K17" s="5"/>
       <c r="L17" s="9">
         <f t="shared" si="1"/>
-        <v>0.97236249272332897</v>
+        <v>0</v>
       </c>
       <c r="M17" s="9">
         <f t="shared" si="2"/>
-        <v>0.97300411864606307</v>
+        <v>0.97264227457795993</v>
       </c>
       <c r="N17" s="9">
         <f t="shared" si="3"/>
-        <v>0.9715957354818241</v>
+        <v>0</v>
       </c>
       <c r="P17" s="5">
         <v>2.5127600000000001</v>
@@ -5487,30 +5455,26 @@
         <v>0.76804600000000001</v>
       </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="27">
-        <v>3.9055212834252402E-2</v>
-      </c>
-      <c r="I18" s="22">
-        <v>3.80746E-2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>3.8125399999999997E-2</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="4"/>
-        <v>3.7975434243599997E-2</v>
-      </c>
+      <c r="H18">
+        <v>1.3618779251700099</v>
+      </c>
+      <c r="I18" s="22"/>
+      <c r="J18" s="32">
+        <f xml:space="preserve"> 1.31449+0.0125614</f>
+        <v>1.3270514</v>
+      </c>
+      <c r="K18" s="2"/>
       <c r="L18" s="11">
         <f t="shared" si="1"/>
-        <v>0.97489162744000257</v>
+        <v>0</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="2"/>
-        <v>0.97619235009169025</v>
+        <v>0.97442757201188768</v>
       </c>
       <c r="N18" s="11">
         <f t="shared" si="3"/>
-        <v>0.97235251040021442</v>
+        <v>0</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="2">
@@ -5538,30 +5502,26 @@
         <v>0.59492599999999995</v>
       </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="28">
-        <v>5.8983323870902299E-2</v>
-      </c>
-      <c r="I19" s="26">
-        <v>5.7466000000000003E-2</v>
-      </c>
-      <c r="J19" s="5">
-        <v>5.76763E-2</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="4"/>
-        <v>5.7744756325199986E-2</v>
-      </c>
+      <c r="H19" s="4">
+        <v>1.34128105403747</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="33">
+        <f>1.29243+0.0122101</f>
+        <v>1.3046400999999999</v>
+      </c>
+      <c r="K19" s="5"/>
       <c r="L19" s="9">
         <f t="shared" si="1"/>
-        <v>0.9742753752870339</v>
+        <v>0</v>
       </c>
       <c r="M19" s="9">
         <f t="shared" si="2"/>
-        <v>0.97784078981776268</v>
+        <v>0.9726821206285029</v>
       </c>
       <c r="N19" s="9">
         <f t="shared" si="3"/>
-        <v>0.97900139455665158</v>
+        <v>0</v>
       </c>
       <c r="P19" s="5">
         <v>4.60677</v>
@@ -5589,30 +5549,26 @@
         <v>0.42067599999999999</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="27">
-        <v>0.103595084893309</v>
-      </c>
-      <c r="I20" s="22">
-        <v>0.10137699999999999</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.101622</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="4"/>
-        <v>0.10128474657560001</v>
-      </c>
+      <c r="H20">
+        <v>1.2896852557910301</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="32">
+        <f xml:space="preserve"> 1.24511+0.0114002</f>
+        <v>1.2565101999999999</v>
+      </c>
+      <c r="K20" s="2"/>
       <c r="L20" s="11">
         <f t="shared" si="1"/>
-        <v>0.97858889834789575</v>
+        <v>0</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="2"/>
-        <v>0.98095387541463919</v>
+        <v>0.97427662629927314</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="3"/>
-        <v>0.97769837902938761</v>
+        <v>0</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="2">
@@ -5640,30 +5596,26 @@
         <v>0.34348000000000001</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="28">
-        <v>0.14519436153500101</v>
-      </c>
-      <c r="I21" s="26">
-        <v>0.14219300000000001</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0.142043</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="4"/>
-        <v>0.14184209068399997</v>
-      </c>
+      <c r="H21" s="4">
+        <v>1.24225887840578</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="33">
+        <f>1.19988+ 0.0105698</f>
+        <v>1.2104498000000001</v>
+      </c>
+      <c r="K21" s="5"/>
       <c r="L21" s="9">
         <f t="shared" si="1"/>
-        <v>0.97932866329470047</v>
+        <v>0</v>
       </c>
       <c r="M21" s="9">
         <f t="shared" si="2"/>
-        <v>0.97829556532578343</v>
+        <v>0.97439416295691827</v>
       </c>
       <c r="N21" s="9">
         <f t="shared" si="3"/>
-        <v>0.9769118386171427</v>
+        <v>0</v>
       </c>
       <c r="P21" s="5">
         <v>11.315899999999999</v>
@@ -5691,30 +5643,26 @@
         <v>0.29746400000000001</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="27">
-        <v>0.185920101577397</v>
-      </c>
-      <c r="I22" s="22">
-        <v>0.18163399999999999</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.181612</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="4"/>
-        <v>0.18159106812</v>
-      </c>
+      <c r="H22">
+        <v>1.1938794039418501</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="32">
+        <f>1.15479+0.00980097</f>
+        <v>1.1645909699999999</v>
+      </c>
+      <c r="K22" s="2"/>
       <c r="L22" s="11">
         <f t="shared" si="1"/>
-        <v>0.97694654025555849</v>
+        <v>0</v>
       </c>
       <c r="M22" s="11">
         <f t="shared" si="2"/>
-        <v>0.97682820985549224</v>
+        <v>0.97546784554189636</v>
       </c>
       <c r="N22" s="11">
         <f t="shared" si="3"/>
-        <v>0.97671562450392246</v>
+        <v>0</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="2">
@@ -5813,7 +5761,7 @@
         <v>0.1</v>
       </c>
       <c r="B27" s="11">
-        <f t="shared" ref="B27:B39" si="5">A27*$Q$5</f>
+        <f t="shared" ref="B27:B39" si="4">A27*$Q$5</f>
         <v>4.0296735505064935E-2</v>
       </c>
       <c r="C27" s="12">
@@ -5830,27 +5778,20 @@
       <c r="H27" s="27">
         <v>3.52725672373683E-5</v>
       </c>
-      <c r="I27" s="22">
-        <v>2.2214699999999999E-5</v>
-      </c>
-      <c r="J27" s="2">
-        <v>2.25088E-5</v>
-      </c>
-      <c r="K27" s="2">
-        <f>P27*$T$4*$W$3*1E-24</f>
-        <v>2.0764465399999998E-5</v>
-      </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
       <c r="L27" s="11">
-        <f t="shared" ref="L27:L39" si="6">I27/H27</f>
-        <v>0.62980105333714986</v>
+        <f t="shared" ref="L27:L39" si="5">I27/H27</f>
+        <v>0</v>
       </c>
       <c r="M27" s="11">
-        <f t="shared" ref="M27:M39" si="7">J27/H27</f>
-        <v>0.63813897776495931</v>
+        <f t="shared" ref="M27:M39" si="6">J27/H27</f>
+        <v>0</v>
       </c>
       <c r="N27" s="11">
-        <f t="shared" ref="N27:N39" si="8">K27/H27</f>
-        <v>0.58868596834090958</v>
+        <f t="shared" ref="N27:N39" si="7">K27/H27</f>
+        <v>0</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="2">
@@ -5863,7 +5804,7 @@
         <v>0.5</v>
       </c>
       <c r="B28" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.20148367752532464</v>
       </c>
       <c r="C28" s="10">
@@ -5879,27 +5820,20 @@
       <c r="H28" s="28">
         <v>1.76088265923015E-4</v>
       </c>
-      <c r="I28" s="26">
-        <v>1.06229E-4</v>
-      </c>
-      <c r="J28" s="5">
-        <v>1.00448E-4</v>
-      </c>
-      <c r="K28" s="5">
-        <f t="shared" ref="K28:K39" si="9">P28*$T$4*$W$3*1E-24</f>
-        <v>1.1061240399999999E-4</v>
-      </c>
+      <c r="I28" s="26"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
       <c r="L28" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
         <f t="shared" si="6"/>
-        <v>0.60327131647967303</v>
-      </c>
-      <c r="M28" s="9">
+        <v>0</v>
+      </c>
+      <c r="N28" s="9">
         <f t="shared" si="7"/>
-        <v>0.57044119023760176</v>
-      </c>
-      <c r="N28" s="9">
-        <f t="shared" si="8"/>
-        <v>0.62816453680314643</v>
+        <v>0</v>
       </c>
       <c r="P28" s="5">
         <v>17.754799999999999</v>
@@ -5911,7 +5845,7 @@
         <v>1.5</v>
       </c>
       <c r="B29" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.60445103257597399</v>
       </c>
       <c r="C29" s="12">
@@ -5928,27 +5862,20 @@
       <c r="H29" s="27">
         <v>5.2684723504348998E-4</v>
       </c>
-      <c r="I29" s="22">
-        <v>3.3353199999999999E-4</v>
-      </c>
-      <c r="J29" s="2">
-        <v>3.2863E-4</v>
-      </c>
-      <c r="K29" s="2">
-        <f t="shared" si="9"/>
-        <v>3.3546182599999996E-4</v>
-      </c>
+      <c r="I29" s="22"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="11">
         <f t="shared" si="6"/>
-        <v>0.63307155815758953</v>
-      </c>
-      <c r="M29" s="11">
+        <v>0</v>
+      </c>
+      <c r="N29" s="11">
         <f t="shared" si="7"/>
-        <v>0.62376715324864973</v>
-      </c>
-      <c r="N29" s="11">
-        <f t="shared" si="8"/>
-        <v>0.63673452888541471</v>
+        <v>0</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="2">
@@ -5961,7 +5888,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.044510325759739</v>
       </c>
       <c r="C30" s="10">
@@ -5977,27 +5904,20 @@
       <c r="H30" s="28">
         <v>5.02535867346246E-3</v>
       </c>
-      <c r="I30" s="26">
-        <v>3.22792E-3</v>
-      </c>
-      <c r="J30" s="5">
-        <v>3.1989399999999999E-3</v>
-      </c>
-      <c r="K30" s="5">
-        <f t="shared" si="9"/>
-        <v>3.1236285499999998E-3</v>
-      </c>
+      <c r="I30" s="26"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
       <c r="L30" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="9">
         <f t="shared" si="6"/>
-        <v>0.64232629146368392</v>
-      </c>
-      <c r="M30" s="9">
+        <v>0</v>
+      </c>
+      <c r="N30" s="9">
         <f t="shared" si="7"/>
-        <v>0.63655953890271044</v>
-      </c>
-      <c r="N30" s="9">
-        <f t="shared" si="8"/>
-        <v>0.62157325535688124</v>
+        <v>0</v>
       </c>
       <c r="P30" s="5">
         <v>501.38499999999999</v>
@@ -6009,7 +5929,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>12.089020651519478</v>
       </c>
       <c r="C31" s="12">
@@ -6026,27 +5946,20 @@
       <c r="H31" s="27">
         <v>9.6096776712520909E-3</v>
       </c>
-      <c r="I31" s="25">
-        <v>6.4084199999999997E-3</v>
-      </c>
-      <c r="J31" s="2">
-        <v>6.4294499999999997E-3</v>
-      </c>
-      <c r="K31" s="2">
-        <f t="shared" si="9"/>
-        <v>6.2577857999999995E-3</v>
-      </c>
+      <c r="I31" s="25"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
       <c r="L31" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="11">
         <f t="shared" si="6"/>
-        <v>0.66687148302290722</v>
-      </c>
-      <c r="M31" s="11">
+        <v>0</v>
+      </c>
+      <c r="N31" s="11">
         <f t="shared" si="7"/>
-        <v>0.66905990189807019</v>
-      </c>
-      <c r="N31" s="11">
-        <f t="shared" si="8"/>
-        <v>0.65119622260802035</v>
+        <v>0</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="2">
@@ -6059,7 +5972,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>24.178041303038956</v>
       </c>
       <c r="C32" s="10">
@@ -6075,27 +5988,20 @@
       <c r="H32" s="28">
         <v>1.7956202904139199E-2</v>
       </c>
-      <c r="I32" s="26">
-        <v>1.27028E-2</v>
-      </c>
-      <c r="J32" s="5">
-        <v>1.26584E-2</v>
-      </c>
-      <c r="K32" s="5">
-        <f t="shared" si="9"/>
-        <v>1.2780408899999998E-2</v>
-      </c>
+      <c r="I32" s="26"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
       <c r="L32" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="9">
         <f t="shared" si="6"/>
-        <v>0.70743241585178329</v>
-      </c>
-      <c r="M32" s="9">
+        <v>0</v>
+      </c>
+      <c r="N32" s="9">
         <f t="shared" si="7"/>
-        <v>0.70495973272177892</v>
-      </c>
-      <c r="N32" s="9">
-        <f t="shared" si="8"/>
-        <v>0.71175453787358933</v>
+        <v>0</v>
       </c>
       <c r="P32" s="5">
         <v>2051.4299999999998</v>
@@ -6108,7 +6014,7 @@
         <v>90</v>
       </c>
       <c r="B33" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>36.267061954558436</v>
       </c>
       <c r="C33" s="12">
@@ -6125,27 +6031,20 @@
       <c r="H33" s="27">
         <v>2.54716677488637E-2</v>
       </c>
-      <c r="I33" s="22">
-        <v>1.8848799999999999E-2</v>
-      </c>
-      <c r="J33" s="2">
-        <v>1.8641399999999999E-2</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="9"/>
-        <v>1.83316504E-2</v>
-      </c>
+      <c r="I33" s="22"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="11">
         <f t="shared" si="6"/>
-        <v>0.73999080805538731</v>
-      </c>
-      <c r="M33" s="11">
+        <v>0</v>
+      </c>
+      <c r="N33" s="11">
         <f t="shared" si="7"/>
-        <v>0.73184842797863514</v>
-      </c>
-      <c r="N33" s="11">
-        <f t="shared" si="8"/>
-        <v>0.71968787363040965</v>
+        <v>0</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="2">
@@ -6160,7 +6059,7 @@
         <v>120</v>
       </c>
       <c r="B34" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>48.356082606077912</v>
       </c>
       <c r="C34" s="10">
@@ -6176,27 +6075,20 @@
       <c r="H34" s="28">
         <v>3.2417642839879697E-2</v>
       </c>
-      <c r="I34" s="26">
-        <v>2.47298E-2</v>
-      </c>
-      <c r="J34" s="5">
-        <v>2.4878500000000001E-2</v>
-      </c>
-      <c r="K34" s="5">
-        <f t="shared" si="9"/>
-        <v>2.4631987099999999E-2</v>
-      </c>
+      <c r="I34" s="26"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
       <c r="L34" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="9">
         <f t="shared" si="6"/>
-        <v>0.76285003577057653</v>
-      </c>
-      <c r="M34" s="9">
+        <v>0</v>
+      </c>
+      <c r="N34" s="9">
         <f t="shared" si="7"/>
-        <v>0.76743704417012226</v>
-      </c>
-      <c r="N34" s="9">
-        <f t="shared" si="8"/>
-        <v>0.75983276210625961</v>
+        <v>0</v>
       </c>
       <c r="P34" s="5">
         <v>3953.77</v>
@@ -6208,7 +6100,7 @@
         <v>150</v>
       </c>
       <c r="B35" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>60.445103257597395</v>
       </c>
       <c r="C35" s="12">
@@ -6225,27 +6117,20 @@
       <c r="H35" s="27">
         <v>3.9055212834252402E-2</v>
       </c>
-      <c r="I35" s="25">
-        <v>3.0672700000000001E-2</v>
-      </c>
-      <c r="J35" s="2">
-        <v>2.95511E-2</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" si="9"/>
-        <v>3.0206154999999998E-2</v>
-      </c>
+      <c r="I35" s="25"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
       <c r="L35" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="11">
         <f t="shared" si="6"/>
-        <v>0.78536763146504407</v>
-      </c>
-      <c r="M35" s="11">
+        <v>0</v>
+      </c>
+      <c r="N35" s="11">
         <f t="shared" si="7"/>
-        <v>0.7566493140214805</v>
-      </c>
-      <c r="N35" s="11">
-        <f t="shared" si="8"/>
-        <v>0.77342185096245186</v>
+        <v>0</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="2">
@@ -6258,7 +6143,7 @@
         <v>250</v>
       </c>
       <c r="B36" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>100.74183876266233</v>
       </c>
       <c r="C36" s="10">
@@ -6274,27 +6159,20 @@
       <c r="H36" s="28">
         <v>5.8983323870902299E-2</v>
       </c>
-      <c r="I36" s="26">
-        <v>4.9196200000000002E-2</v>
-      </c>
-      <c r="J36" s="5">
-        <v>4.8565799999999999E-2</v>
-      </c>
-      <c r="K36" s="5">
-        <f t="shared" si="9"/>
-        <v>4.8230853299999994E-2</v>
-      </c>
+      <c r="I36" s="26"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
       <c r="L36" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="9">
         <f t="shared" si="6"/>
-        <v>0.834069644967389</v>
-      </c>
-      <c r="M36" s="9">
+        <v>0</v>
+      </c>
+      <c r="N36" s="9">
         <f t="shared" si="7"/>
-        <v>0.82338187834745813</v>
-      </c>
-      <c r="N36" s="9">
-        <f t="shared" si="8"/>
-        <v>0.81770321058141104</v>
+        <v>0</v>
       </c>
       <c r="P36" s="5">
         <v>7741.71</v>
@@ -6306,7 +6184,7 @@
         <v>500</v>
       </c>
       <c r="B37" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>201.48367752532465</v>
       </c>
       <c r="C37" s="12">
@@ -6323,27 +6201,20 @@
       <c r="H37" s="27">
         <v>0.103595084893309</v>
       </c>
-      <c r="I37" s="25">
-        <v>9.2448600000000006E-2</v>
-      </c>
-      <c r="J37" s="2">
-        <v>8.9643600000000004E-2</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="9"/>
-        <v>8.8566302999999999E-2</v>
-      </c>
+      <c r="I37" s="25"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="11">
         <f t="shared" si="6"/>
-        <v>0.89240334225519879</v>
-      </c>
-      <c r="M37" s="11">
+        <v>0</v>
+      </c>
+      <c r="N37" s="11">
         <f t="shared" si="7"/>
-        <v>0.86532676808289299</v>
-      </c>
-      <c r="N37" s="11">
-        <f t="shared" si="8"/>
-        <v>0.85492765502545887</v>
+        <v>0</v>
       </c>
       <c r="O37" s="4"/>
       <c r="P37" s="2">
@@ -6356,7 +6227,7 @@
         <v>750</v>
       </c>
       <c r="B38" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>302.22551628798698</v>
       </c>
       <c r="C38" s="10">
@@ -6372,27 +6243,20 @@
       <c r="H38" s="28">
         <v>0.14519436153500101</v>
       </c>
-      <c r="I38" s="26">
-        <v>0.133441</v>
-      </c>
-      <c r="J38" s="5">
-        <v>0.124949</v>
-      </c>
-      <c r="K38" s="5">
-        <f t="shared" si="9"/>
-        <v>0.12434955399999999</v>
-      </c>
+      <c r="I38" s="26"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
       <c r="L38" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="9">
         <f t="shared" si="6"/>
-        <v>0.91905084046829388</v>
-      </c>
-      <c r="M38" s="9">
+        <v>0</v>
+      </c>
+      <c r="N38" s="9">
         <f t="shared" si="7"/>
-        <v>0.86056372078801013</v>
-      </c>
-      <c r="N38" s="9">
-        <f t="shared" si="8"/>
-        <v>0.85643514448750746</v>
+        <v>0</v>
       </c>
       <c r="P38" s="5">
         <v>19959.8</v>
@@ -6404,7 +6268,7 @@
         <v>1000</v>
       </c>
       <c r="B39" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>402.9673550506493</v>
       </c>
       <c r="C39" s="12">
@@ -6421,27 +6285,20 @@
       <c r="H39" s="27">
         <v>0.185920101577397</v>
       </c>
-      <c r="I39" s="22">
-        <v>0.17522299999999999</v>
-      </c>
-      <c r="J39" s="2">
-        <v>0.1593</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="9"/>
-        <v>0.16219431200000001</v>
-      </c>
+      <c r="I39" s="22"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
       <c r="L39" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="11">
         <f t="shared" si="6"/>
-        <v>0.94246398594536107</v>
-      </c>
-      <c r="M39" s="11">
+        <v>0</v>
+      </c>
+      <c r="N39" s="11">
         <f t="shared" si="7"/>
-        <v>0.85681966957018219</v>
-      </c>
-      <c r="N39" s="11">
-        <f t="shared" si="8"/>
-        <v>0.87238717397365373</v>
+        <v>0</v>
       </c>
       <c r="O39" s="4"/>
       <c r="P39" s="2">
@@ -6545,7 +6402,7 @@
         <v>0.1</v>
       </c>
       <c r="B44" s="11">
-        <f t="shared" ref="B44:B56" si="10">A44*$Q$5</f>
+        <f t="shared" ref="B44:B56" si="8">A44*$Q$5</f>
         <v>4.0296735505064935E-2</v>
       </c>
       <c r="C44" s="12">
@@ -6568,7 +6425,7 @@
         <v>1.3791474000000001</v>
       </c>
       <c r="K44" s="29">
-        <f t="shared" ref="K44:K53" si="11">P44*$T$4*$W$3*1E-24</f>
+        <f t="shared" ref="K44:K53" si="9">P44*$T$4*$W$3*1E-24</f>
         <v>1.3430197899999997E-8</v>
       </c>
       <c r="L44" s="11">
@@ -6580,7 +6437,7 @@
         <v>0.98215385902659358</v>
       </c>
       <c r="N44" s="11">
-        <f t="shared" ref="N44:N56" si="12">K44/H44</f>
+        <f t="shared" ref="N44:N56" si="10">K44/H44</f>
         <v>9.5642573774027705E-9</v>
       </c>
       <c r="O44" s="4"/>
@@ -6594,7 +6451,7 @@
         <v>0.5</v>
       </c>
       <c r="B45" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0.20148367752532464</v>
       </c>
       <c r="C45" s="10">
@@ -6616,19 +6473,19 @@
         <v>1.3790180999999999</v>
       </c>
       <c r="K45" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6.7190549999999991E-8</v>
       </c>
       <c r="L45" s="9">
-        <f t="shared" ref="L45:L56" si="13">I45/H45</f>
+        <f t="shared" ref="L45:L56" si="11">I45/H45</f>
         <v>0</v>
       </c>
       <c r="M45" s="33">
-        <f t="shared" ref="M45:M56" si="14">J45/H45</f>
+        <f t="shared" ref="M45:M56" si="12">J45/H45</f>
         <v>0.98203818000196974</v>
       </c>
       <c r="N45" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4.7848309920900489E-8</v>
       </c>
       <c r="P45" s="30">
@@ -6641,7 +6498,7 @@
         <v>1.5</v>
       </c>
       <c r="B46" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0.60445103257597399</v>
       </c>
       <c r="C46" s="12">
@@ -6664,19 +6521,19 @@
         <v>1.3789032000000001</v>
       </c>
       <c r="K46" s="29">
+        <f t="shared" si="9"/>
+        <v>2.01536762E-7</v>
+      </c>
+      <c r="L46" s="11">
         <f t="shared" si="11"/>
-        <v>2.01536762E-7</v>
-      </c>
-      <c r="L46" s="11">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M46" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.98233124644332637</v>
       </c>
       <c r="N46" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.4357487793168658E-7</v>
       </c>
       <c r="O46" s="4"/>
@@ -6690,7 +6547,7 @@
         <v>15</v>
       </c>
       <c r="B47" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6.044510325759739</v>
       </c>
       <c r="C47" s="10">
@@ -6712,19 +6569,19 @@
         <v>1.375659</v>
       </c>
       <c r="K47" s="30">
+        <f t="shared" si="9"/>
+        <v>2.0174608999999998E-6</v>
+      </c>
+      <c r="L47" s="9">
         <f t="shared" si="11"/>
-        <v>2.0174608999999998E-6</v>
-      </c>
-      <c r="L47" s="9">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M47" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.98414421045326572</v>
       </c>
       <c r="N47" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.4432882455251154E-6</v>
       </c>
       <c r="P47" s="30">
@@ -6737,7 +6594,7 @@
         <v>30</v>
       </c>
       <c r="B48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12.089020651519478</v>
       </c>
       <c r="C48" s="12">
@@ -6760,19 +6617,19 @@
         <v>1.3743595</v>
       </c>
       <c r="K48" s="29">
+        <f t="shared" si="9"/>
+        <v>4.0416128199999999E-6</v>
+      </c>
+      <c r="L48" s="11">
         <f t="shared" si="11"/>
-        <v>4.0416128199999999E-6</v>
-      </c>
-      <c r="L48" s="11">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M48" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.98620843151639703</v>
       </c>
       <c r="N48" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2.9001674161736885E-6</v>
       </c>
       <c r="O48" s="4"/>
@@ -6786,7 +6643,7 @@
         <v>60</v>
       </c>
       <c r="B49" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>24.178041303038956</v>
       </c>
       <c r="C49" s="10">
@@ -6808,19 +6665,19 @@
         <v>1.3686853999999999</v>
       </c>
       <c r="K49" s="30">
+        <f t="shared" si="9"/>
+        <v>8.1020526999999998E-6</v>
+      </c>
+      <c r="L49" s="9">
         <f t="shared" si="11"/>
-        <v>8.1020526999999998E-6</v>
-      </c>
-      <c r="L49" s="9">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M49" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.9879632515229031</v>
       </c>
       <c r="N49" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>5.8483347082550277E-6</v>
       </c>
       <c r="P49" s="30">
@@ -6833,7 +6690,7 @@
         <v>90</v>
       </c>
       <c r="B50" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>36.267061954558436</v>
       </c>
       <c r="C50" s="12">
@@ -6856,19 +6713,19 @@
         <v>1.3632628</v>
       </c>
       <c r="K50" s="29">
+        <f t="shared" si="9"/>
+        <v>1.21776564E-5</v>
+      </c>
+      <c r="L50" s="11">
         <f t="shared" si="11"/>
-        <v>1.21776564E-5</v>
-      </c>
-      <c r="L50" s="11">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M50" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.98890099734312431</v>
       </c>
       <c r="N50" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8.8335840743706049E-6</v>
       </c>
       <c r="O50" s="4"/>
@@ -6882,7 +6739,7 @@
         <v>120</v>
       </c>
       <c r="B51" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>48.356082606077912</v>
       </c>
       <c r="C51" s="10">
@@ -6904,19 +6761,19 @@
         <v>1.357774</v>
       </c>
       <c r="K51" s="30">
+        <f t="shared" si="9"/>
+        <v>1.6280859E-5</v>
+      </c>
+      <c r="L51" s="9">
         <f t="shared" si="11"/>
-        <v>1.6280859E-5</v>
-      </c>
-      <c r="L51" s="9">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M51" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.99111928758233259</v>
       </c>
       <c r="N51" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.1884358791159948E-5</v>
       </c>
       <c r="P51" s="30">
@@ -6929,7 +6786,7 @@
         <v>150</v>
       </c>
       <c r="B52" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>60.445103257597395</v>
       </c>
       <c r="C52" s="12">
@@ -6952,19 +6809,19 @@
         <v>1.3511147999999999</v>
       </c>
       <c r="K52" s="29">
+        <f t="shared" si="9"/>
+        <v>2.0403748399999997E-5</v>
+      </c>
+      <c r="L52" s="11">
         <f t="shared" si="11"/>
-        <v>2.0403748399999997E-5</v>
-      </c>
-      <c r="L52" s="11">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M52" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.9920968502601536</v>
       </c>
       <c r="N52" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.4982068526775552E-5</v>
       </c>
       <c r="O52" s="4"/>
@@ -6978,7 +6835,7 @@
         <v>250</v>
       </c>
       <c r="B53" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>100.74183876266233</v>
       </c>
       <c r="C53" s="10">
@@ -7000,19 +6857,19 @@
         <v>1.3364325000000001</v>
       </c>
       <c r="K53" s="30">
+        <f t="shared" si="9"/>
+        <v>3.4383432299999996E-5</v>
+      </c>
+      <c r="L53" s="9">
         <f t="shared" si="11"/>
-        <v>3.4383432299999996E-5</v>
-      </c>
-      <c r="L53" s="9">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M53" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.99638513194317113</v>
       </c>
       <c r="N53" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2.5634770726463613E-5</v>
       </c>
       <c r="P53" s="30">
@@ -7025,7 +6882,7 @@
         <v>500</v>
       </c>
       <c r="B54" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>201.48367752532465</v>
       </c>
       <c r="C54" s="12">
@@ -7052,15 +6909,15 @@
         <v>7.059213E-5</v>
       </c>
       <c r="L54" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M54" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.0083240032099037</v>
       </c>
       <c r="N54" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>5.473593629377598E-5</v>
       </c>
       <c r="O54" s="4"/>
@@ -7074,7 +6931,7 @@
         <v>750</v>
       </c>
       <c r="B55" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>302.22551628798698</v>
       </c>
       <c r="C55" s="10">
@@ -7100,15 +6957,15 @@
         <v>1.09394439E-4</v>
       </c>
       <c r="L55" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M55" s="33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.0206371812187167</v>
       </c>
       <c r="N55" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8.8060903328288914E-5</v>
       </c>
       <c r="P55" s="30">
@@ -7121,7 +6978,7 @@
         <v>1000</v>
       </c>
       <c r="B56" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>402.9673550506493</v>
       </c>
       <c r="C56" s="12">
@@ -7148,15 +7005,15 @@
         <v>1.5084512099999999E-4</v>
       </c>
       <c r="L56" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M56" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.0391633324972136</v>
       </c>
       <c r="N56" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.263487086735497E-4</v>
       </c>
       <c r="O56" s="4"/>

</xml_diff>

<commit_message>
FLiBe 30% Li6 U238 done
</commit_message>
<xml_diff>
--- a/Jupyter/Wedge/wedge_data_2025-12-31.xlsx
+++ b/Jupyter/Wedge/wedge_data_2025-12-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\Jupyter\Wedge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA05213-BEA7-4978-A3AA-349D2210DDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94E60D6-2905-475C-AB82-69F19C78A886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4869,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22416C2-1180-4450-A3B0-0B08DD9AEC85}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>